<commit_message>
packaging program, adding comments
</commit_message>
<xml_diff>
--- a/CompletedProgram/Outputs/ptx 200 7d.xlsx
+++ b/CompletedProgram/Outputs/ptx 200 7d.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\CompletedProgram\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F754126-8046-454A-9067-787031459F2B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B400E8A4-D06A-4AA3-83CE-3D33E9299DA6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11118" windowHeight="7938" xr2:uid="{0A043804-813C-44D3-A04F-8360F25351D3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7932" xr2:uid="{DFE0AC71-4B89-41E2-B4F2-13B186EC4154}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>Group</t>
   </si>
@@ -300,6 +300,21 @@
   </si>
   <si>
     <t>ptx 200nM 8.2.4.txt</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Mean NCV (m/s)</t>
+  </si>
+  <si>
+    <t>Median NCV (m/s)</t>
+  </si>
+  <si>
+    <t>ctrl</t>
+  </si>
+  <si>
+    <t>ptx200nm</t>
   </si>
 </sst>
 </file>
@@ -650,16 +665,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1CAE1E-3AC5-4A43-8EF5-A841ABE8FDCC}">
-  <dimension ref="A1:E86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6213E9-C9B8-4413-A39D-F24A64D1FF0E}">
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E86"/>
+      <selection activeCell="G1" sqref="G1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -675,8 +690,17 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -692,8 +716,17 @@
       <c r="E2">
         <v>0.31385999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2">
+        <v>0.34858</v>
+      </c>
+      <c r="I2">
+        <v>0.34336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -709,8 +742,17 @@
       <c r="E3">
         <v>0.30149999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3">
+        <v>0.28210000000000002</v>
+      </c>
+      <c r="I3">
+        <v>0.27984999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -727,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -744,7 +786,7 @@
         <v>0.17496</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -761,7 +803,7 @@
         <v>0.30567</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -778,7 +820,7 @@
         <v>0.16811999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -795,7 +837,7 @@
         <v>0.51031000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -812,7 +854,7 @@
         <v>0.54281000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -829,7 +871,7 @@
         <v>0.38261000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -846,7 +888,7 @@
         <v>0.14815</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -863,7 +905,7 @@
         <v>0.40354000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -880,7 +922,7 @@
         <v>0.26346000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -897,7 +939,7 @@
         <v>0.43933</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -914,7 +956,7 @@
         <v>0.31061</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
removed extraneous inputs/outputs from betterBaseline and added comprehensive comments
</commit_message>
<xml_diff>
--- a/CompletedProgram/Outputs/ptx 200 7d.xlsx
+++ b/CompletedProgram/Outputs/ptx 200 7d.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\CompletedProgram\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B400E8A4-D06A-4AA3-83CE-3D33E9299DA6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3744AD16-7CB2-4F7B-B83F-2D09DFBE4CD9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7932" xr2:uid="{DFE0AC71-4B89-41E2-B4F2-13B186EC4154}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7932" xr2:uid="{D8A44B22-FE5F-499A-970D-CD736E2B5D16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6213E9-C9B8-4413-A39D-F24A64D1FF0E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0625DBD7-65C3-4D03-ABDD-31E457E90179}">
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>